<commit_message>
Minor fixes to OceanAccounts file to match template.
</commit_message>
<xml_diff>
--- a/crosswalks/OceanAccounts-IUCNGET/OceanAccounts-IUCNGET.xlsx
+++ b/crosswalks/OceanAccounts-IUCNGET/OceanAccounts-IUCNGET.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dropbox\Documents\NEAP\Ecosystem-Typology\crosswalks\OceanAccounts-IUCNGET\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67EC94C0-A587-4858-BDE8-6A55FCB2AE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6845D978-2CEF-4B70-A68E-21AAE3350182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{D01AE75A-5DB4-4EB9-9B33-8751D4445479}"/>
   </bookViews>
   <sheets>
     <sheet name="OceanAccountsInfo" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
   <si>
     <t>Realm</t>
   </si>
@@ -168,25 +168,16 @@
     <t>semapv:ManualMappingCuration</t>
   </si>
   <si>
-    <t>Reviewer1</t>
-  </si>
-  <si>
-    <t>Reviewer2</t>
-  </si>
-  <si>
     <t>skos:closeMatch</t>
   </si>
   <si>
     <t>skos:exactMatch</t>
   </si>
   <si>
-    <t>https://orcid.org/0009-0001-6090-9959</t>
-  </si>
-  <si>
-    <t>https://orcid.org/0000-0002-2568-5945</t>
-  </si>
-  <si>
-    <t>https://orcid.org/0000-0003-4254-8683</t>
+    <t>reviewer_id</t>
+  </si>
+  <si>
+    <t>orcid:0000-0002-2568-5945</t>
   </si>
   <si>
     <t>author_label</t>
@@ -216,9 +207,6 @@
     <t>see email from Toni Cannard for review comments</t>
   </si>
   <si>
-    <t>High</t>
-  </si>
-  <si>
     <t>creator_id: https://orcid.org/0000-0002-3884-3420</t>
   </si>
   <si>
@@ -259,6 +247,15 @@
   </si>
   <si>
     <t>ocean: TBA</t>
+  </si>
+  <si>
+    <t>orcid:0009-0001-6090-9959</t>
+  </si>
+  <si>
+    <t>orcid:0000-0003-4254-8683</t>
+  </si>
+  <si>
+    <t>high</t>
   </si>
 </sst>
 </file>
@@ -297,12 +294,10 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -328,9 +323,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -342,13 +336,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -712,7 +705,7 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -726,7 +719,7 @@
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -740,7 +733,7 @@
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -754,7 +747,7 @@
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -769,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692E3A1F-E8D6-4D8F-836E-084FC2E29426}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -780,52 +773,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -835,10 +828,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ACFEC63-F603-4D93-B073-540A32B07BA6}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +875,7 @@
         <v>24</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>25</v>
@@ -891,13 +884,13 @@
         <v>26</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>27</v>
@@ -905,16 +898,16 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -922,43 +915,43 @@
       <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>33</v>
+      <c r="G2" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="H2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I2" s="4">
         <v>45292</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="K2" t="s">
-        <v>39</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="L2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" t="s">
+        <v>57</v>
       </c>
       <c r="N2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -966,40 +959,43 @@
       <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>33</v>
+      <c r="G3" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I3" s="4">
         <v>45292</v>
       </c>
+      <c r="J3" t="s">
+        <v>58</v>
+      </c>
       <c r="K3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>57</v>
       </c>
       <c r="N3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
@@ -1007,40 +1003,43 @@
       <c r="F4" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>33</v>
+      <c r="G4" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="H4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I4" s="4">
         <v>45292</v>
       </c>
+      <c r="J4" t="s">
+        <v>58</v>
+      </c>
       <c r="K4" t="s">
-        <v>39</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="L4" t="s">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s">
+        <v>57</v>
       </c>
       <c r="N4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
@@ -1048,34 +1047,40 @@
       <c r="F5" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>33</v>
+      <c r="G5" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="H5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I5" s="4">
         <v>45292</v>
       </c>
+      <c r="J5" t="s">
+        <v>58</v>
+      </c>
       <c r="K5" t="s">
-        <v>39</v>
-      </c>
-      <c r="L5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
+        <v>57</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
-      </c>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G7" s="6"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2:G5" r:id="rId1" display="https://orcid.org/0009-0001-6090-9959" xr:uid="{F1564EBB-DE64-4F09-91EA-7C41E7F5661F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>